<commit_message>
New update file excel
</commit_message>
<xml_diff>
--- a/Huan/Web-job-data/ITViec-Hoang.xlsx
+++ b/Huan/Web-job-data/ITViec-Hoang.xlsx
@@ -5,25 +5,25 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\study\study\Ngon ngu lap trinh\Python\Thuc hanh\Scraping\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Minh Hoang\source\repos\Teamb_Scraping_data\Huan\Web-job-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D17BD0F-A8CF-41A7-9347-4CF4BAD9A692}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D55FDD88-45DA-4804-9653-522084FB07E9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="687" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="687" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data scientist" sheetId="2" r:id="rId1"/>
     <sheet name="Data Engineers" sheetId="6" r:id="rId2"/>
     <sheet name="Data Analyst" sheetId="3" r:id="rId3"/>
-    <sheet name="Business Analyst" sheetId="4" r:id="rId4"/>
+    <sheet name="BA" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="277">
   <si>
     <t>Title</t>
   </si>
@@ -2277,6 +2277,18 @@
 Attractive salary and bonusHealth insurance and Social insurance regulated by Vietnam Labor LawProfessional, dynamic working environment
 Apply Now
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -2321,7 +2333,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -2344,11 +2356,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2362,6 +2385,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2701,13 +2727,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17808979-C60A-4EA1-A703-BD015F5794DF}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="2" width="14.85546875" style="3" customWidth="1"/>
@@ -2719,10 +2745,10 @@
     <col min="9" max="9" width="19.7109375" style="3" customWidth="1"/>
     <col min="10" max="10" width="9.140625" style="3"/>
     <col min="11" max="11" width="17" style="3" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="3"/>
+    <col min="14" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2753,8 +2779,14 @@
       <c r="K1" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="171" x14ac:dyDescent="0.2">
+      <c r="L1" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="171.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>0</v>
       </c>
@@ -2788,8 +2820,11 @@
       <c r="K2" s="3" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="171" x14ac:dyDescent="0.2">
+      <c r="L2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="171.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -2823,8 +2858,11 @@
       <c r="K3" s="3" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="171" x14ac:dyDescent="0.2">
+      <c r="L3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="171.75" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -2858,8 +2896,11 @@
       <c r="K4" s="3" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="171" x14ac:dyDescent="0.2">
+      <c r="L4" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="171.75" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -2893,8 +2934,11 @@
       <c r="K5" s="3" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="171" x14ac:dyDescent="0.2">
+      <c r="L5" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="171.75" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -2927,6 +2971,199 @@
       </c>
       <c r="K6" s="3" t="s">
         <v>228</v>
+      </c>
+      <c r="L6" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L7" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L8" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L9" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L10" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L11" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L12" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L13" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L15" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L16" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="17" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L17" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="18" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L18" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="19" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L19" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="20" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L20" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="21" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L21" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="22" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L22" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="24" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L24" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="25" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L25" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="26" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L26" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="27" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L27" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="28" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L28" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="29" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L29" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="30" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L30" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="31" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L31" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="32" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L32" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="33" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L33" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="34" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L34" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="35" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L35" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="36" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L36" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="37" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L37" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="38" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L38" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="39" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L39" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="40" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L40" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="41" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L41" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="42" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L42" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="43" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L43" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="44" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L44" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="45" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L45" t="s">
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -2937,15 +3174,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{248389D4-0EC5-4C20-9A41-0EEEEA5CD4CB}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:M45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="L1" sqref="L1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2976,8 +3213,14 @@
       <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+      <c r="L1" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3011,8 +3254,11 @@
       <c r="K2" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="195" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="195" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>3</v>
       </c>
@@ -3045,6 +3291,214 @@
       </c>
       <c r="K3" t="s">
         <v>231</v>
+      </c>
+      <c r="L3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L5" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L6" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L7" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L8" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L9" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L10" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L11" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L12" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L13" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L15" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L16" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="17" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L17" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="18" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L18" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="19" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L19" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="20" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L20" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="21" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L21" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="22" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L22" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="24" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L24" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="25" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L25" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="26" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L26" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="27" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L27" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="28" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L28" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="29" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L29" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="30" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L30" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="31" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L31" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="32" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L32" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="33" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L33" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="34" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L34" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="35" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L35" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="36" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L36" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="37" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L37" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="38" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L38" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="39" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L39" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="40" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L40" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="41" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L41" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="42" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L42" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="43" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L43" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="44" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L44" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="45" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L45" t="s">
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -3054,19 +3508,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47B3F11E-0E62-43E0-B110-F5E36ECC4736}">
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
-    <col min="3" max="3" width="35.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3097,8 +3551,14 @@
       <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+      <c r="L1" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3132,8 +3592,11 @@
       <c r="K2" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3167,8 +3630,11 @@
       <c r="K3" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3202,8 +3668,11 @@
       <c r="K4" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>8</v>
       </c>
@@ -3237,8 +3706,11 @@
       <c r="K5" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+      <c r="L5" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>9</v>
       </c>
@@ -3272,8 +3744,11 @@
       <c r="K6" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+      <c r="L6" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>10</v>
       </c>
@@ -3307,8 +3782,11 @@
       <c r="K7" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+      <c r="L7" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>11</v>
       </c>
@@ -3342,8 +3820,11 @@
       <c r="K8" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+      <c r="L8" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>12</v>
       </c>
@@ -3377,8 +3858,11 @@
       <c r="K9" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>13</v>
       </c>
@@ -3412,8 +3896,11 @@
       <c r="K10" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>15</v>
       </c>
@@ -3447,8 +3934,11 @@
       <c r="K11" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>16</v>
       </c>
@@ -3482,8 +3972,11 @@
       <c r="K12" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>17</v>
       </c>
@@ -3517,8 +4010,11 @@
       <c r="K13" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+      <c r="L13" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>18</v>
       </c>
@@ -3552,8 +4048,11 @@
       <c r="K14" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+      <c r="L14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>19</v>
       </c>
@@ -3587,8 +4086,11 @@
       <c r="K15" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>22</v>
       </c>
@@ -3622,8 +4124,11 @@
       <c r="K16" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>24</v>
       </c>
@@ -3657,8 +4162,11 @@
       <c r="K17" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+      <c r="L17" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="180" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>40</v>
       </c>
@@ -3692,8 +4200,11 @@
       <c r="K18" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43</v>
       </c>
@@ -3727,8 +4238,11 @@
       <c r="K19" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>44</v>
       </c>
@@ -3762,8 +4276,11 @@
       <c r="K20" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+      <c r="L20" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="180" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>45</v>
       </c>
@@ -3797,8 +4314,11 @@
       <c r="K21" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+      <c r="L21" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="180" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>46</v>
       </c>
@@ -3832,8 +4352,11 @@
       <c r="K22" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="L22" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>47</v>
       </c>
@@ -3868,7 +4391,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="180" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>48</v>
       </c>
@@ -3902,8 +4425,11 @@
       <c r="K24" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>49</v>
       </c>
@@ -3937,8 +4463,11 @@
       <c r="K25" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>50</v>
       </c>
@@ -3972,8 +4501,11 @@
       <c r="K26" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="L26" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>51</v>
       </c>
@@ -4007,8 +4539,11 @@
       <c r="K27" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+      <c r="L27" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="180" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>52</v>
       </c>
@@ -4042,8 +4577,11 @@
       <c r="K28" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L28" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>53</v>
       </c>
@@ -4077,8 +4615,11 @@
       <c r="K29" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+      <c r="L29" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="180" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>54</v>
       </c>
@@ -4112,8 +4653,11 @@
       <c r="K30" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L30" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>55</v>
       </c>
@@ -4147,8 +4691,11 @@
       <c r="K31" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+      <c r="L31" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="180" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>56</v>
       </c>
@@ -4182,8 +4729,11 @@
       <c r="K32" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L32" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>57</v>
       </c>
@@ -4217,8 +4767,11 @@
       <c r="K33" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L33" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>58</v>
       </c>
@@ -4252,8 +4805,11 @@
       <c r="K34" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L34" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>59</v>
       </c>
@@ -4287,8 +4843,11 @@
       <c r="K35" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L35" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>60</v>
       </c>
@@ -4322,8 +4881,11 @@
       <c r="K36" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L36" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>61</v>
       </c>
@@ -4357,8 +4919,11 @@
       <c r="K37" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L37" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>62</v>
       </c>
@@ -4392,8 +4957,11 @@
       <c r="K38" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L38" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>63</v>
       </c>
@@ -4427,8 +4995,11 @@
       <c r="K39" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L39" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>64</v>
       </c>
@@ -4462,8 +5033,11 @@
       <c r="K40" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+      <c r="L40" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="180" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>65</v>
       </c>
@@ -4496,6 +5070,29 @@
       </c>
       <c r="K41" t="s">
         <v>264</v>
+      </c>
+      <c r="L41" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L42" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L43" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L44" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L45" t="s">
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -4505,18 +5102,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E845F8B2-C964-49F1-A794-DB36B02B18B2}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="43.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4547,8 +5144,14 @@
       <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+      <c r="L1" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4582,8 +5185,11 @@
       <c r="K2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4617,8 +5223,11 @@
       <c r="K3" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -4652,8 +5261,11 @@
       <c r="K4" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -4687,8 +5299,11 @@
       <c r="K5" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -4722,8 +5337,11 @@
       <c r="K6" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -4757,8 +5375,11 @@
       <c r="K7" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L7" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -4792,10 +5413,13 @@
       <c r="K8" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
@@ -4827,10 +5451,13 @@
       <c r="K9" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>43</v>
@@ -4862,10 +5489,13 @@
       <c r="K10" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
@@ -4896,6 +5526,174 @@
       </c>
       <c r="K11" t="s">
         <v>228</v>
+      </c>
+      <c r="L11" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L12" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L13" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L15" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L16" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="17" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L17" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="18" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L18" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="19" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L19" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="20" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L20" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="21" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L21" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="22" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L22" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="24" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L24" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="25" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L25" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="26" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L26" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="27" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L27" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="28" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L28" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="29" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L29" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="30" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L30" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="31" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L31" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="32" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L32" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="33" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L33" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="34" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L34" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="35" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L35" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="36" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L36" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="37" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L37" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="38" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L38" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="39" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L39" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="40" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L40" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="41" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L41" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="42" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L42" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="43" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L43" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="44" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L44" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="45" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L45" t="s">
+        <v>273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>